<commit_message>
Pushing update to data
</commit_message>
<xml_diff>
--- a/data-raw/SARS/Revenue.xlsx
+++ b/data-raw/SARS/Revenue.xlsx
@@ -1549,10 +1549,10 @@
   <dimension ref="A1:AO74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="AB47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="AE2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AM79" sqref="AM79"/>
+      <selection pane="bottomRight" activeCell="AP8" sqref="AP8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changed SARS data structure
</commit_message>
<xml_diff>
--- a/data-raw/SARS/Revenue.xlsx
+++ b/data-raw/SARS/Revenue.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Annual" sheetId="2" r:id="rId1"/>
@@ -1548,7 +1548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="AE2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -8846,11 +8846,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:HZ91"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="AQ2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="AR29" sqref="AR29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23733,7 +23733,7 @@
         <v>10203827</v>
       </c>
       <c r="AR28" s="7">
-        <v>79993417</v>
+        <v>7993417</v>
       </c>
       <c r="AS28" s="7">
         <v>9274594</v>

</xml_diff>